<commit_message>
Adding IFrame embedded youtube
</commit_message>
<xml_diff>
--- a/com.automation.aws.testing/Extent-Report/IOFile.xlsx
+++ b/com.automation.aws.testing/Extent-Report/IOFile.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,19 +19,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>This 1st</t>
   </si>
   <si>
     <t>This is 2nd</t>
   </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Hello Again</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,10 +359,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>